<commit_message>
16 - Title Changed.
</commit_message>
<xml_diff>
--- a/Project Details-for-DEV.xlsx
+++ b/Project Details-for-DEV.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8621918A-B665-499F-A001-4F479AA41AD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -284,7 +285,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -342,7 +343,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -387,6 +388,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -435,7 +442,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -470,6 +477,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -567,6 +578,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -602,6 +630,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -777,11 +822,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A4:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,18 +1162,19 @@
       </c>
     </row>
     <row r="24" spans="1:8" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="8">
+      <c r="A24" s="18">
         <v>16</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="18" t="s">
         <v>60</v>
       </c>
+      <c r="E24" s="18"/>
       <c r="F24" s="8" t="s">
         <v>52</v>
       </c>
@@ -1436,36 +1482,36 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C9" r:id="rId1"/>
-    <hyperlink ref="C10" r:id="rId2"/>
-    <hyperlink ref="C11" r:id="rId3"/>
-    <hyperlink ref="C12" r:id="rId4"/>
-    <hyperlink ref="C13" r:id="rId5"/>
-    <hyperlink ref="C14" r:id="rId6"/>
-    <hyperlink ref="C15" r:id="rId7"/>
-    <hyperlink ref="C16" r:id="rId8"/>
-    <hyperlink ref="C17" r:id="rId9"/>
-    <hyperlink ref="C18" r:id="rId10"/>
-    <hyperlink ref="C19" r:id="rId11"/>
-    <hyperlink ref="C20" r:id="rId12"/>
-    <hyperlink ref="C21" r:id="rId13"/>
-    <hyperlink ref="C22" r:id="rId14"/>
-    <hyperlink ref="C23" r:id="rId15"/>
-    <hyperlink ref="C24" r:id="rId16"/>
-    <hyperlink ref="C25" r:id="rId17"/>
-    <hyperlink ref="C26" r:id="rId18"/>
-    <hyperlink ref="C27" r:id="rId19"/>
-    <hyperlink ref="C28" r:id="rId20"/>
-    <hyperlink ref="C29" r:id="rId21"/>
-    <hyperlink ref="C30" r:id="rId22"/>
-    <hyperlink ref="C31" r:id="rId23"/>
-    <hyperlink ref="C32" r:id="rId24"/>
-    <hyperlink ref="C33" r:id="rId25"/>
-    <hyperlink ref="C34" r:id="rId26"/>
-    <hyperlink ref="C35" r:id="rId27"/>
-    <hyperlink ref="C36" r:id="rId28"/>
-    <hyperlink ref="C37" r:id="rId29"/>
-    <hyperlink ref="C38" r:id="rId30"/>
+    <hyperlink ref="C9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C10" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C11" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C12" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C13" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C14" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C15" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C16" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C17" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="C18" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="C19" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="C20" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="C21" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="C22" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="C23" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="C24" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="C25" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="C26" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="C27" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="C28" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="C29" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="C30" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="C31" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="C32" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="C33" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="C34" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="C35" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="C36" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="C37" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="C38" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId31"/>
@@ -1473,7 +1519,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C5:E1008"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
@@ -6563,7 +6609,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E22" r:id="rId1"/>
+    <hyperlink ref="E22" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Added extra column for Final Changes.
</commit_message>
<xml_diff>
--- a/Project Details-for-DEV.xlsx
+++ b/Project Details-for-DEV.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="89">
   <si>
     <t>Category</t>
   </si>
@@ -279,6 +279,9 @@
   </si>
   <si>
     <t>Done but changes</t>
+  </si>
+  <si>
+    <t>URL Change and Final changes</t>
   </si>
 </sst>
 </file>
@@ -788,10 +791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:H38"/>
+  <dimension ref="A4:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,15 +804,16 @@
     <col min="3" max="3" width="53.5703125" customWidth="1"/>
     <col min="4" max="4" width="21.42578125" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" customWidth="1"/>
-    <col min="6" max="6" width="24.5703125" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="31.42578125" customWidth="1"/>
+    <col min="7" max="7" width="24.5703125" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G4" s="15"/>
-    </row>
-    <row r="8" spans="1:8" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H4" s="15"/>
+    </row>
+    <row r="8" spans="1:9" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>22</v>
       </c>
@@ -826,16 +830,19 @@
         <v>3</v>
       </c>
       <c r="F8" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="G8" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="H8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="I8" s="10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>1</v>
       </c>
@@ -851,11 +858,14 @@
       <c r="E9" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>2</v>
       </c>
@@ -871,11 +881,14 @@
       <c r="E10" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>3</v>
       </c>
@@ -891,11 +904,14 @@
       <c r="E11" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
         <v>4</v>
       </c>
@@ -905,14 +921,14 @@
       <c r="C12" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="G12" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="9">
+      <c r="H12" s="9">
         <v>44006</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8">
         <v>5</v>
       </c>
@@ -928,11 +944,14 @@
       <c r="E13" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8">
         <v>6</v>
       </c>
@@ -948,11 +967,14 @@
       <c r="E14" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F14" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
         <v>7</v>
       </c>
@@ -968,11 +990,14 @@
       <c r="E15" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="F15" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <v>8</v>
       </c>
@@ -988,11 +1013,14 @@
       <c r="E16" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <v>9</v>
       </c>
@@ -1008,11 +1036,14 @@
       <c r="E17" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8">
         <v>10</v>
       </c>
@@ -1028,11 +1059,14 @@
       <c r="E18" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G18" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8">
         <v>11</v>
       </c>
@@ -1048,11 +1082,14 @@
       <c r="E19" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G19" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8">
         <v>12</v>
       </c>
@@ -1068,11 +1105,14 @@
       <c r="E20" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F20" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G20" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8">
         <v>13</v>
       </c>
@@ -1088,11 +1128,14 @@
       <c r="E21" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F21" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G21" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7">
         <v>14</v>
       </c>
@@ -1102,11 +1145,11 @@
       <c r="C22" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="G22" s="7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8">
         <v>15</v>
       </c>
@@ -1119,14 +1162,14 @@
       <c r="D23" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F23" s="11" t="s">
+      <c r="G23" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="G23" s="9">
+      <c r="H23" s="9">
         <v>43997</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="18">
         <v>16</v>
       </c>
@@ -1140,17 +1183,18 @@
         <v>60</v>
       </c>
       <c r="E24" s="18"/>
-      <c r="F24" s="8" t="s">
+      <c r="F24" s="18"/>
+      <c r="G24" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="G24" s="9">
+      <c r="H24" s="9">
         <v>43996</v>
       </c>
-      <c r="H24" s="9">
+      <c r="I24" s="9">
         <v>43998</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8">
         <v>17</v>
       </c>
@@ -1163,17 +1207,17 @@
       <c r="D25" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="G25" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G25" s="9">
+      <c r="H25" s="9">
         <v>43996</v>
       </c>
-      <c r="H25" s="9">
+      <c r="I25" s="9">
         <v>43999</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="8">
         <v>18</v>
       </c>
@@ -1186,17 +1230,17 @@
       <c r="D26" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="G26" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="G26" s="9">
+      <c r="H26" s="9">
         <v>43998</v>
       </c>
-      <c r="H26" s="9">
+      <c r="I26" s="9">
         <v>43999</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="8">
         <v>19</v>
       </c>
@@ -1209,17 +1253,17 @@
       <c r="D27" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="G27" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="G27" s="9">
+      <c r="H27" s="9">
         <v>43998</v>
       </c>
-      <c r="H27" s="9">
+      <c r="I27" s="9">
         <v>44001</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="8">
         <v>20</v>
       </c>
@@ -1232,17 +1276,17 @@
       <c r="D28" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F28" s="8" t="s">
+      <c r="G28" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="G28" s="9">
+      <c r="H28" s="9">
         <v>43996</v>
       </c>
-      <c r="H28" s="9">
+      <c r="I28" s="9">
         <v>43998</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="8">
         <v>21</v>
       </c>
@@ -1252,14 +1296,14 @@
       <c r="C29" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="F29" s="8" t="s">
+      <c r="G29" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="H29" s="9">
+      <c r="I29" s="9">
         <v>44006</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8">
         <v>22</v>
       </c>
@@ -1272,17 +1316,17 @@
       <c r="D30" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="G30" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="G30" s="9">
+      <c r="H30" s="9">
         <v>43998</v>
       </c>
-      <c r="H30" s="9">
+      <c r="I30" s="9">
         <v>43999</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="8">
         <v>23</v>
       </c>
@@ -1295,17 +1339,17 @@
       <c r="D31" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F31" s="8" t="s">
+      <c r="G31" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="G31" s="9">
+      <c r="H31" s="9">
         <v>43996</v>
       </c>
-      <c r="H31" s="9">
+      <c r="I31" s="9">
         <v>43998</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="8">
         <v>24</v>
       </c>
@@ -1318,14 +1362,14 @@
       <c r="D32" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F32" s="8" t="s">
+      <c r="G32" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="G32" s="9">
+      <c r="H32" s="9">
         <v>43998</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="8">
         <v>25</v>
       </c>
@@ -1338,14 +1382,14 @@
       <c r="D33" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F33" s="8" t="s">
+      <c r="G33" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="G33" s="9">
+      <c r="H33" s="9">
         <v>43996</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="8">
         <v>26</v>
       </c>
@@ -1355,14 +1399,14 @@
       <c r="C34" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="F34" s="8" t="s">
+      <c r="G34" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="G34" s="9">
+      <c r="H34" s="9">
         <v>44000</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="8">
         <v>27</v>
       </c>
@@ -1375,14 +1419,14 @@
       <c r="D35" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F35" s="8" t="s">
+      <c r="G35" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="G35" s="9">
+      <c r="H35" s="9">
         <v>44000</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="8">
         <v>28</v>
       </c>
@@ -1395,14 +1439,14 @@
       <c r="D36" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F36" s="8" t="s">
+      <c r="G36" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="G36" s="9">
+      <c r="H36" s="9">
         <v>44000</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="8">
         <v>29</v>
       </c>
@@ -1415,14 +1459,14 @@
       <c r="D37" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="F37" s="8" t="s">
+      <c r="G37" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="G37" s="9">
+      <c r="H37" s="9">
         <v>44000</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="8">
         <v>30</v>
       </c>
@@ -1435,10 +1479,10 @@
       <c r="D38" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F38" s="8" t="s">
+      <c r="G38" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="G38" s="9">
+      <c r="H38" s="9">
         <v>44000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
21 + 24 - Done- excel sheet updated
</commit_message>
<xml_diff>
--- a/Project Details-for-DEV.xlsx
+++ b/Project Details-for-DEV.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="89">
   <si>
     <t>Category</t>
   </si>
@@ -794,7 +794,7 @@
   <dimension ref="A4:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1296,6 +1296,9 @@
       <c r="C29" s="17" t="s">
         <v>77</v>
       </c>
+      <c r="D29" s="8" t="s">
+        <v>60</v>
+      </c>
       <c r="G29" s="8" t="s">
         <v>52</v>
       </c>
@@ -1360,7 +1363,7 @@
         <v>80</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
Main menu,mobile menu, Javascript, and Style css changed..
1) mobile menu,
2) Main Menu
3) Button Hover
4) Style css
5) Gallery
6) AOS

All are changes in both 16 and 25 HTML.
</commit_message>
<xml_diff>
--- a/Project Details-for-DEV.xlsx
+++ b/Project Details-for-DEV.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237D1426-6EB2-43ED-A052-2559AEC87459}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="89">
   <si>
     <t>Category</t>
   </si>
@@ -287,7 +288,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -580,6 +581,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -615,6 +633,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -790,11 +825,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A4:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1182,7 +1217,9 @@
       <c r="D24" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E24" s="18"/>
+      <c r="E24" s="18" t="s">
+        <v>60</v>
+      </c>
       <c r="F24" s="18"/>
       <c r="G24" s="8" t="s">
         <v>52</v>
@@ -1370,18 +1407,20 @@
       </c>
     </row>
     <row r="33" spans="1:8" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="8">
+      <c r="A33" s="18">
         <v>25</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="17" t="s">
+      <c r="C33" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="18" t="s">
         <v>60</v>
       </c>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
       <c r="G33" s="8" t="s">
         <v>52</v>
       </c>
@@ -1488,36 +1527,36 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C9" r:id="rId1"/>
-    <hyperlink ref="C10" r:id="rId2"/>
-    <hyperlink ref="C11" r:id="rId3"/>
-    <hyperlink ref="C12" r:id="rId4"/>
-    <hyperlink ref="C13" r:id="rId5"/>
-    <hyperlink ref="C14" r:id="rId6"/>
-    <hyperlink ref="C15" r:id="rId7"/>
-    <hyperlink ref="C16" r:id="rId8"/>
-    <hyperlink ref="C17" r:id="rId9"/>
-    <hyperlink ref="C18" r:id="rId10"/>
-    <hyperlink ref="C19" r:id="rId11"/>
-    <hyperlink ref="C20" r:id="rId12"/>
-    <hyperlink ref="C21" r:id="rId13"/>
-    <hyperlink ref="C22" r:id="rId14"/>
-    <hyperlink ref="C23" r:id="rId15"/>
-    <hyperlink ref="C24" r:id="rId16"/>
-    <hyperlink ref="C25" r:id="rId17"/>
-    <hyperlink ref="C26" r:id="rId18"/>
-    <hyperlink ref="C27" r:id="rId19"/>
-    <hyperlink ref="C28" r:id="rId20"/>
-    <hyperlink ref="C29" r:id="rId21"/>
-    <hyperlink ref="C30" r:id="rId22"/>
-    <hyperlink ref="C31" r:id="rId23"/>
-    <hyperlink ref="C32" r:id="rId24"/>
-    <hyperlink ref="C33" r:id="rId25"/>
-    <hyperlink ref="C34" r:id="rId26"/>
-    <hyperlink ref="C35" r:id="rId27"/>
-    <hyperlink ref="C36" r:id="rId28"/>
-    <hyperlink ref="C37" r:id="rId29"/>
-    <hyperlink ref="C38" r:id="rId30"/>
+    <hyperlink ref="C9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C10" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C11" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C12" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C13" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C14" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C15" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C16" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C17" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="C18" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="C19" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="C20" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="C21" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="C22" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="C23" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="C24" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="C25" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="C26" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="C27" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="C28" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="C29" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="C30" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="C31" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="C32" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="C33" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="C34" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="C35" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="C36" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="C37" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="C38" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId31"/>
@@ -1525,7 +1564,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C5:E1008"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
@@ -6615,7 +6654,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E22" r:id="rId1"/>
+    <hyperlink ref="E22" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>